<commit_message>
Fix en el nombre de Kai'Sa y Bel'Veth
</commit_message>
<xml_diff>
--- a/lolchamps.xlsx
+++ b/lolchamps.xlsx
@@ -147,406 +147,406 @@
     <t xml:space="preserve">Graves</t>
   </si>
   <si>
+    <t xml:space="preserve">Kai'Sa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Karma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gangplank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hecarim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kalista</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leona</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Garen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ivern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kog'Maw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lulu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gnar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jarvan IV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fizz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lucian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gragas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Karthus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Galio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miss Fortune</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maokai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kayn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samira</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Morgana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bel'Veth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gwen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kha'Zix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heimerdinger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sivir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nami</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kindred</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Irelia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tristana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nautilus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Illaoi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lee Sin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kassadin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Twitch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pantheon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lillia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Katarina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ziggs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pyke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Master Yi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LeBlanc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rakan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jayce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nidalee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lissandra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kennen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nocturne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Renata Glasc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nunu &amp; Willump</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Malzahar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Senna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Malphite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olaf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neeko</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seraphine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mordekaiser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poppy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orianna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sona</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nasus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rammus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qiyana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soraka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rek'Sai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ryze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Swain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ornn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rengar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quinn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sejuani</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sylas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thresh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Renekton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shaco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Syndra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vel'Koz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Riven</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shyvana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taliyah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xerath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rumble</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skarner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Talon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yuumi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sett</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Twisted Fate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zilean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Veigar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zyra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Singed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trundle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Udyr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viktor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vladimir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tahm Kench</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viego</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teemo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volibear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yasuo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tryndamere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warwick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Urgot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wukong</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vayne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xin Zhao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zoe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yorick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kayle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nunu and Willump</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Varus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xayah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zeri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANY-WIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOP-WIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JG-WIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MID-WIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC-WIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUPP-WIN</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kai'sa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Karma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gangplank</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hecarim</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Corki</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kalista</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leona</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Garen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ivern</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kog'Maw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lulu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gnar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jarvan IV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fizz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lucian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gragas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Karthus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Galio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Miss Fortune</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maokai</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kayn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Samira</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Morgana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bel'Veth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gwen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kha'Zix</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Heimerdinger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sivir</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nami</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kindred</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Irelia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tristana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nautilus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Illaoi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lee Sin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kassadin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Twitch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pantheon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lillia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Katarina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ziggs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pyke</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jax</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Master Yi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LeBlanc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rakan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jayce</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nidalee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lissandra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kennen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nocturne</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Renata Glasc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kled</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nunu &amp; Willump</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Malzahar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Senna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Malphite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Olaf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Neeko</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Seraphine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mordekaiser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Poppy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Orianna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sona</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nasus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rammus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Qiyana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Soraka</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rek'Sai</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ryze</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Swain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ornn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rengar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Taric</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quinn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sejuani</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sylas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thresh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Renekton</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shaco</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Syndra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vel'Koz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Riven</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shyvana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Taliyah</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Xerath</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rumble</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Skarner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Talon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yuumi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sett</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Twisted Fate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zilean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Veigar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zyra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Singed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trundle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Udyr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Viktor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vladimir</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tahm Kench</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Viego</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Teemo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volibear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yasuo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tryndamere</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Warwick</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Urgot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wukong</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vayne</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Xin Zhao</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zoe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zac</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yorick</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kai'Sa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kayle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nunu and Willump</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Varus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Xayah</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zeri</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANY-WIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOP-WIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JG-WIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MID-WIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADC-WIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SUPP-WIN</t>
   </si>
 </sst>
 </file>
@@ -768,16 +768,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -864,10 +864,10 @@
   <dimension ref="A1:M1001"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N11" activeCellId="0" sqref="N11"/>
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.63"/>
@@ -1174,7 +1174,7 @@
       <c r="J8" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="K8" s="18" t="s">
+      <c r="K8" s="11" t="s">
         <v>31</v>
       </c>
       <c r="L8" s="12" t="s">
@@ -2550,10 +2550,10 @@
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="17" t="s">
-        <v>163</v>
+        <v>41</v>
       </c>
       <c r="H54" s="8" t="s">
-        <v>163</v>
+        <v>41</v>
       </c>
       <c r="I54" s="9"/>
       <c r="J54" s="10"/>
@@ -2628,10 +2628,10 @@
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H60" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I60" s="9"/>
       <c r="J60" s="10"/>
@@ -2992,10 +2992,10 @@
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H88" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I88" s="9"/>
       <c r="J88" s="10"/>
@@ -3627,10 +3627,10 @@
     </row>
     <row r="137" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A137" s="17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H137" s="17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I137" s="9"/>
       <c r="J137" s="10"/>
@@ -3752,10 +3752,10 @@
     </row>
     <row r="149" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A149" s="17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H149" s="17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3824,10 +3824,10 @@
     </row>
     <row r="158" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A158" s="17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H158" s="17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4723,7 +4723,7 @@
       <selection pane="topLeft" activeCell="K34" activeCellId="0" sqref="K34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.63"/>
@@ -4761,78 +4761,78 @@
         <v>5</v>
       </c>
       <c r="H1" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="I1" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="J1" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="K1" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="L1" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="M1" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="M1" s="13" t="s">
-        <v>174</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="19" t="n">
+      <c r="A2" s="18" t="n">
         <f aca="false">ROWS(A$3:A$250) - COUNTBLANK(A$3:A$250)</f>
         <v>160</v>
       </c>
-      <c r="B2" s="19" t="n">
+      <c r="B2" s="18" t="n">
         <f aca="false">ROWS(B$3:B$250) - COUNTBLANK(B$3:B$250)</f>
         <v>45</v>
       </c>
-      <c r="C2" s="19" t="n">
+      <c r="C2" s="18" t="n">
         <f aca="false">ROWS(C$3:C$250) - COUNTBLANK(C$3:C$250)</f>
         <v>42</v>
       </c>
-      <c r="D2" s="19" t="n">
+      <c r="D2" s="18" t="n">
         <f aca="false">ROWS(D$3:D$250) - COUNTBLANK(D$3:D$250)</f>
         <v>40</v>
       </c>
-      <c r="E2" s="19" t="n">
+      <c r="E2" s="18" t="n">
         <f aca="false">ROWS(E$3:E$250) - COUNTBLANK(E$3:E$250)</f>
         <v>17</v>
       </c>
-      <c r="F2" s="19" t="n">
+      <c r="F2" s="18" t="n">
         <f aca="false">ROWS(F$3:F$250) - COUNTBLANK(F$3:F$250)</f>
         <v>32</v>
       </c>
-      <c r="G2" s="19" t="n">
+      <c r="G2" s="18" t="n">
         <f aca="false">ROWS(G$3:G$250) - COUNTBLANK(G$3:G$250)</f>
         <v>0</v>
       </c>
-      <c r="H2" s="19" t="n">
+      <c r="H2" s="18" t="n">
         <f aca="false">ROWS(H$3:H$250) - COUNTBLANK(H$3:H$250)</f>
         <v>132</v>
       </c>
-      <c r="I2" s="19" t="n">
+      <c r="I2" s="18" t="n">
         <f aca="false">ROWS(I$3:I$250) - COUNTBLANK(I$3:I$250)</f>
         <v>34</v>
       </c>
-      <c r="J2" s="19" t="n">
+      <c r="J2" s="18" t="n">
         <f aca="false">ROWS(J$3:J$250) - COUNTBLANK(J$3:J$250)</f>
         <v>34</v>
       </c>
-      <c r="K2" s="19" t="n">
+      <c r="K2" s="18" t="n">
         <f aca="false">ROWS(K$3:K$250) - COUNTBLANK(K$3:K$250)</f>
         <v>0</v>
       </c>
-      <c r="L2" s="19" t="n">
+      <c r="L2" s="18" t="n">
         <f aca="false">ROWS(L$3:L$250) - COUNTBLANK(L$3:L$250)</f>
         <v>14</v>
       </c>
-      <c r="M2" s="19" t="n">
+      <c r="M2" s="18" t="n">
         <f aca="false">ROWS(M$3:M$250) - COUNTBLANK(M$3:M$250)</f>
         <v>31</v>
       </c>
-      <c r="N2" s="20"/>
+      <c r="N2" s="19"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
@@ -4898,7 +4898,7 @@
       <c r="J4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="18"/>
+      <c r="K4" s="20"/>
       <c r="L4" s="12" t="s">
         <v>17</v>
       </c>
@@ -4934,7 +4934,7 @@
       <c r="J5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="K5" s="18"/>
+      <c r="K5" s="20"/>
       <c r="L5" s="12" t="s">
         <v>22</v>
       </c>
@@ -4970,7 +4970,7 @@
       <c r="J6" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="18"/>
+      <c r="K6" s="20"/>
       <c r="L6" s="12" t="s">
         <v>37</v>
       </c>
@@ -5006,9 +5006,9 @@
       <c r="J7" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K7" s="18"/>
+      <c r="K7" s="20"/>
       <c r="L7" s="12" t="s">
-        <v>41</v>
+        <v>174</v>
       </c>
       <c r="M7" s="13" t="s">
         <v>28</v>
@@ -5042,7 +5042,7 @@
       <c r="J8" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="K8" s="18"/>
+      <c r="K8" s="20"/>
       <c r="L8" s="12" t="s">
         <v>46</v>
       </c>
@@ -5078,7 +5078,7 @@
       <c r="J9" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="K9" s="18"/>
+      <c r="K9" s="20"/>
       <c r="L9" s="12" t="s">
         <v>50</v>
       </c>
@@ -5100,7 +5100,7 @@
         <v>19</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>41</v>
+        <v>174</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>42</v>
@@ -5114,7 +5114,7 @@
       <c r="J10" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="K10" s="18"/>
+      <c r="K10" s="20"/>
       <c r="L10" s="12" t="s">
         <v>55</v>
       </c>
@@ -5150,7 +5150,7 @@
       <c r="J11" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="K11" s="18"/>
+      <c r="K11" s="20"/>
       <c r="L11" s="12" t="s">
         <v>60</v>
       </c>
@@ -5186,7 +5186,7 @@
       <c r="J12" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="K12" s="18"/>
+      <c r="K12" s="20"/>
       <c r="L12" s="12" t="s">
         <v>63</v>
       </c>
@@ -5222,7 +5222,7 @@
       <c r="J13" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="K13" s="18"/>
+      <c r="K13" s="20"/>
       <c r="L13" s="12" t="s">
         <v>69</v>
       </c>
@@ -5258,7 +5258,7 @@
       <c r="J14" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="K14" s="18"/>
+      <c r="K14" s="20"/>
       <c r="L14" s="12" t="s">
         <v>73</v>
       </c>
@@ -5294,7 +5294,7 @@
       <c r="J15" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="K15" s="18"/>
+      <c r="K15" s="20"/>
       <c r="L15" s="12" t="s">
         <v>78</v>
       </c>
@@ -5330,7 +5330,7 @@
       <c r="J16" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="K16" s="18"/>
+      <c r="K16" s="20"/>
       <c r="L16" s="12" t="s">
         <v>82</v>
       </c>
@@ -5366,7 +5366,7 @@
       <c r="J17" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="K17" s="18"/>
+      <c r="K17" s="20"/>
       <c r="L17" s="12"/>
       <c r="M17" s="13" t="s">
         <v>74</v>
@@ -5400,7 +5400,7 @@
       <c r="J18" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="K18" s="18"/>
+      <c r="K18" s="20"/>
       <c r="L18" s="12"/>
       <c r="M18" s="13" t="s">
         <v>83</v>
@@ -5434,7 +5434,7 @@
       <c r="J19" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="K19" s="18"/>
+      <c r="K19" s="20"/>
       <c r="L19" s="12"/>
       <c r="M19" s="13" t="s">
         <v>87</v>
@@ -5466,7 +5466,7 @@
       <c r="J20" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="K20" s="18"/>
+      <c r="K20" s="20"/>
       <c r="L20" s="12"/>
       <c r="M20" s="13" t="s">
         <v>91</v>
@@ -5498,7 +5498,7 @@
       <c r="J21" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="K21" s="18"/>
+      <c r="K21" s="20"/>
       <c r="L21" s="12"/>
       <c r="M21" s="13" t="s">
         <v>94</v>
@@ -5530,7 +5530,7 @@
       <c r="J22" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="K22" s="18"/>
+      <c r="K22" s="20"/>
       <c r="L22" s="12"/>
       <c r="M22" s="13" t="s">
         <v>98</v>
@@ -5562,7 +5562,7 @@
       <c r="J23" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="K23" s="18"/>
+      <c r="K23" s="20"/>
       <c r="L23" s="12"/>
       <c r="M23" s="13" t="s">
         <v>102</v>
@@ -5594,7 +5594,7 @@
       <c r="J24" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="K24" s="18"/>
+      <c r="K24" s="20"/>
       <c r="L24" s="12"/>
       <c r="M24" s="13" t="s">
         <v>106</v>
@@ -5626,7 +5626,7 @@
       <c r="J25" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="K25" s="18"/>
+      <c r="K25" s="20"/>
       <c r="L25" s="12"/>
       <c r="M25" s="13" t="s">
         <v>110</v>
@@ -5658,7 +5658,7 @@
       <c r="J26" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="K26" s="18"/>
+      <c r="K26" s="20"/>
       <c r="L26" s="12"/>
       <c r="M26" s="13" t="s">
         <v>113</v>
@@ -5690,7 +5690,7 @@
       <c r="J27" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="K27" s="18"/>
+      <c r="K27" s="20"/>
       <c r="L27" s="12"/>
       <c r="M27" s="13" t="s">
         <v>116</v>
@@ -5722,7 +5722,7 @@
       <c r="J28" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="K28" s="18"/>
+      <c r="K28" s="20"/>
       <c r="L28" s="12"/>
       <c r="M28" s="13" t="s">
         <v>120</v>
@@ -5754,7 +5754,7 @@
       <c r="J29" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="K29" s="18"/>
+      <c r="K29" s="20"/>
       <c r="L29" s="12"/>
       <c r="M29" s="13" t="s">
         <v>124</v>
@@ -5786,7 +5786,7 @@
       <c r="J30" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="K30" s="18"/>
+      <c r="K30" s="20"/>
       <c r="L30" s="12"/>
       <c r="M30" s="13" t="s">
         <v>128</v>
@@ -5818,7 +5818,7 @@
       <c r="J31" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="K31" s="18"/>
+      <c r="K31" s="20"/>
       <c r="L31" s="12"/>
       <c r="M31" s="13" t="s">
         <v>132</v>
@@ -5850,7 +5850,7 @@
       <c r="J32" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="K32" s="18"/>
+      <c r="K32" s="20"/>
       <c r="L32" s="12"/>
       <c r="M32" s="13" t="s">
         <v>135</v>
@@ -5882,7 +5882,7 @@
       <c r="J33" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="K33" s="18"/>
+      <c r="K33" s="20"/>
       <c r="L33" s="12"/>
       <c r="M33" s="13" t="s">
         <v>138</v>
@@ -5914,7 +5914,7 @@
       <c r="J34" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="K34" s="18"/>
+      <c r="K34" s="20"/>
       <c r="L34" s="12"/>
       <c r="M34" s="13"/>
     </row>
@@ -6154,7 +6154,7 @@
       <c r="E44" s="6"/>
       <c r="F44" s="7"/>
       <c r="H44" s="8" t="s">
-        <v>163</v>
+        <v>41</v>
       </c>
       <c r="I44" s="9"/>
       <c r="J44" s="10"/>
@@ -6253,7 +6253,7 @@
         <v>84</v>
       </c>
       <c r="H50" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I50" s="9"/>
       <c r="J50" s="10"/>
@@ -6302,7 +6302,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="17" t="s">
-        <v>163</v>
+        <v>41</v>
       </c>
       <c r="H54" s="8" t="s">
         <v>95</v>
@@ -6380,7 +6380,7 @@
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H60" s="8" t="s">
         <v>90</v>
@@ -6565,7 +6565,7 @@
         <v>56</v>
       </c>
       <c r="H74" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I74" s="9"/>
       <c r="J74" s="10"/>
@@ -6744,7 +6744,7 @@
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H88" s="8" t="s">
         <v>63</v>
@@ -7076,7 +7076,7 @@
         <v>136</v>
       </c>
       <c r="H113" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I113" s="9"/>
       <c r="J113" s="10"/>
@@ -7216,7 +7216,7 @@
         <v>123</v>
       </c>
       <c r="H123" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I123" s="9"/>
       <c r="J123" s="10"/>
@@ -7328,7 +7328,7 @@
         <v>140</v>
       </c>
       <c r="H131" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I131" s="9"/>
       <c r="J131" s="10"/>
@@ -7405,7 +7405,7 @@
     </row>
     <row r="137" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A137" s="17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H137" s="8"/>
       <c r="I137" s="9"/>
@@ -7527,7 +7527,7 @@
     </row>
     <row r="149" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A149" s="17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7572,7 +7572,7 @@
     </row>
     <row r="158" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A158" s="17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8457,7 +8457,7 @@
       <selection pane="topLeft" activeCell="K42" activeCellId="0" sqref="K42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.63"/>
@@ -8495,22 +8495,22 @@
         <v>5</v>
       </c>
       <c r="H1" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="I1" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="J1" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="K1" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="L1" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="M1" s="13" t="s">
         <v>173</v>
-      </c>
-      <c r="M1" s="13" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8844,7 +8844,7 @@
         <v>19</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>41</v>
+        <v>174</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>42</v>
@@ -10130,7 +10130,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="17" t="s">
-        <v>163</v>
+        <v>41</v>
       </c>
       <c r="H54" s="8" t="s">
         <v>42</v>
@@ -10185,7 +10185,7 @@
         <v>77</v>
       </c>
       <c r="H58" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I58" s="9"/>
       <c r="J58" s="10"/>
@@ -10208,7 +10208,7 @@
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H60" s="8" t="s">
         <v>92</v>
@@ -10497,7 +10497,7 @@
         <v>70</v>
       </c>
       <c r="H82" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I82" s="9"/>
       <c r="J82" s="10"/>
@@ -10572,7 +10572,7 @@
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H88" s="8" t="s">
         <v>83</v>
@@ -11069,7 +11069,7 @@
         <v>131</v>
       </c>
       <c r="H126" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I126" s="9"/>
       <c r="J126" s="10"/>
@@ -11207,7 +11207,7 @@
     </row>
     <row r="137" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A137" s="17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H137" s="17" t="s">
         <v>156</v>
@@ -11222,7 +11222,7 @@
         <v>157</v>
       </c>
       <c r="H138" s="17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I138" s="9"/>
       <c r="J138" s="10"/>
@@ -11319,7 +11319,7 @@
         <v>153</v>
       </c>
       <c r="H147" s="17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11332,7 +11332,7 @@
     </row>
     <row r="149" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A149" s="17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H149" s="17" t="s">
         <v>135</v>
@@ -11383,7 +11383,7 @@
     </row>
     <row r="158" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A158" s="17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
posibilidad de cambiar de linea y escoger una si no se menciona
</commit_message>
<xml_diff>
--- a/lolchamps.xlsx
+++ b/lolchamps.xlsx
@@ -530,7 +530,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -554,6 +554,14 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -660,7 +668,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -730,6 +738,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -813,10 +829,10 @@
   <dimension ref="A1:M1001"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3:K42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.63"/>
@@ -911,7 +927,7 @@
         <v>42</v>
       </c>
       <c r="K2" s="2" t="n">
-        <f aca="false">ROWS(K3:K325)-COUNTBLANK(K3:K325)</f>
+        <f aca="false">ROWS(K3:K287)-COUNTBLANK(K3:K287)</f>
         <v>40</v>
       </c>
       <c r="L2" s="2" t="n">
@@ -951,7 +967,7 @@
       <c r="J3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="K3" s="5" t="s">
         <v>8</v>
       </c>
       <c r="L3" s="12" t="s">
@@ -989,7 +1005,7 @@
       <c r="J4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="K4" s="5" t="s">
         <v>11</v>
       </c>
       <c r="L4" s="12" t="s">
@@ -1027,7 +1043,7 @@
       <c r="J5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="K5" s="11" t="s">
+      <c r="K5" s="5" t="s">
         <v>16</v>
       </c>
       <c r="L5" s="12" t="s">
@@ -1065,7 +1081,7 @@
       <c r="J6" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="K6" s="5" t="s">
         <v>21</v>
       </c>
       <c r="L6" s="12" t="s">
@@ -1103,7 +1119,7 @@
       <c r="J7" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K7" s="11" t="s">
+      <c r="K7" s="5" t="s">
         <v>26</v>
       </c>
       <c r="L7" s="12" t="s">
@@ -1141,7 +1157,7 @@
       <c r="J8" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="K8" s="11" t="s">
+      <c r="K8" s="5" t="s">
         <v>31</v>
       </c>
       <c r="L8" s="12" t="s">
@@ -1179,7 +1195,7 @@
       <c r="J9" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="K9" s="11" t="s">
+      <c r="K9" s="5" t="s">
         <v>36</v>
       </c>
       <c r="L9" s="12" t="s">
@@ -1217,7 +1233,7 @@
       <c r="J10" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="K10" s="11" t="s">
+      <c r="K10" s="5" t="s">
         <v>19</v>
       </c>
       <c r="L10" s="12" t="s">
@@ -1255,7 +1271,7 @@
       <c r="J11" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="K11" s="11" t="s">
+      <c r="K11" s="5" t="s">
         <v>45</v>
       </c>
       <c r="L11" s="12" t="s">
@@ -1293,7 +1309,7 @@
       <c r="J12" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="K12" s="11" t="s">
+      <c r="K12" s="5" t="s">
         <v>20</v>
       </c>
       <c r="L12" s="12" t="s">
@@ -1331,7 +1347,7 @@
       <c r="J13" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="K13" s="11" t="s">
+      <c r="K13" s="5" t="s">
         <v>54</v>
       </c>
       <c r="L13" s="12" t="s">
@@ -1369,7 +1385,7 @@
       <c r="J14" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="K14" s="11" t="s">
+      <c r="K14" s="5" t="s">
         <v>59</v>
       </c>
       <c r="L14" s="12" t="s">
@@ -1407,7 +1423,7 @@
       <c r="J15" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="K15" s="11" t="s">
+      <c r="K15" s="5" t="s">
         <v>43</v>
       </c>
       <c r="L15" s="12" t="s">
@@ -1445,7 +1461,7 @@
       <c r="J16" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="K16" s="11" t="s">
+      <c r="K16" s="5" t="s">
         <v>67</v>
       </c>
       <c r="L16" s="12" t="s">
@@ -1483,7 +1499,7 @@
       <c r="J17" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="K17" s="11" t="s">
+      <c r="K17" s="5" t="s">
         <v>71</v>
       </c>
       <c r="L17" s="12" t="s">
@@ -1521,7 +1537,7 @@
       <c r="J18" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="K18" s="11" t="s">
+      <c r="K18" s="5" t="s">
         <v>76</v>
       </c>
       <c r="L18" s="12" t="s">
@@ -1559,7 +1575,7 @@
       <c r="J19" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="K19" s="11" t="s">
+      <c r="K19" s="5" t="s">
         <v>80</v>
       </c>
       <c r="L19" s="12" t="s">
@@ -1595,7 +1611,7 @@
       <c r="J20" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="K20" s="11" t="s">
+      <c r="K20" s="5" t="s">
         <v>85</v>
       </c>
       <c r="L20" s="12"/>
@@ -1629,7 +1645,7 @@
       <c r="J21" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="K21" s="11" t="s">
+      <c r="K21" s="5" t="s">
         <v>89</v>
       </c>
       <c r="L21" s="12"/>
@@ -1663,7 +1679,7 @@
       <c r="J22" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="K22" s="11" t="s">
+      <c r="K22" s="5" t="s">
         <v>56</v>
       </c>
       <c r="L22" s="12"/>
@@ -1697,7 +1713,7 @@
       <c r="J23" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="K23" s="11" t="s">
+      <c r="K23" s="5" t="s">
         <v>96</v>
       </c>
       <c r="L23" s="12"/>
@@ -1731,7 +1747,7 @@
       <c r="J24" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="K24" s="11" t="s">
+      <c r="K24" s="5" t="s">
         <v>100</v>
       </c>
       <c r="L24" s="12"/>
@@ -1765,7 +1781,7 @@
       <c r="J25" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="K25" s="11" t="s">
+      <c r="K25" s="5" t="s">
         <v>104</v>
       </c>
       <c r="L25" s="12"/>
@@ -1799,7 +1815,7 @@
       <c r="J26" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="K26" s="11" t="s">
+      <c r="K26" s="5" t="s">
         <v>108</v>
       </c>
       <c r="L26" s="12"/>
@@ -1833,7 +1849,7 @@
       <c r="J27" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="K27" s="11" t="s">
+      <c r="K27" s="5" t="s">
         <v>111</v>
       </c>
       <c r="L27" s="12"/>
@@ -1867,7 +1883,7 @@
       <c r="J28" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="K28" s="11" t="s">
+      <c r="K28" s="5" t="s">
         <v>112</v>
       </c>
       <c r="L28" s="12"/>
@@ -1901,7 +1917,7 @@
       <c r="J29" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="K29" s="11" t="s">
+      <c r="K29" s="5" t="s">
         <v>118</v>
       </c>
       <c r="L29" s="12"/>
@@ -1935,7 +1951,7 @@
       <c r="J30" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="K30" s="11" t="s">
+      <c r="K30" s="5" t="s">
         <v>122</v>
       </c>
       <c r="L30" s="12"/>
@@ -1969,7 +1985,7 @@
       <c r="J31" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="K31" s="11" t="s">
+      <c r="K31" s="5" t="s">
         <v>126</v>
       </c>
       <c r="L31" s="12"/>
@@ -2003,7 +2019,7 @@
       <c r="J32" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="K32" s="11" t="s">
+      <c r="K32" s="5" t="s">
         <v>130</v>
       </c>
       <c r="L32" s="12"/>
@@ -2037,7 +2053,7 @@
       <c r="J33" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="K33" s="11" t="s">
+      <c r="K33" s="5" t="s">
         <v>133</v>
       </c>
       <c r="L33" s="12"/>
@@ -2071,7 +2087,7 @@
       <c r="J34" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="K34" s="11" t="s">
+      <c r="K34" s="5" t="s">
         <v>136</v>
       </c>
       <c r="L34" s="12"/>
@@ -2103,10 +2119,10 @@
       <c r="J35" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="K35" s="11" t="s">
+      <c r="K35" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="L35" s="12"/>
+      <c r="L35" s="18"/>
       <c r="M35" s="13"/>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2133,7 +2149,7 @@
       <c r="J36" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="K36" s="11" t="s">
+      <c r="K36" s="5" t="s">
         <v>143</v>
       </c>
       <c r="L36" s="12"/>
@@ -2163,7 +2179,7 @@
       <c r="J37" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="K37" s="11" t="s">
+      <c r="K37" s="5" t="s">
         <v>145</v>
       </c>
       <c r="L37" s="12"/>
@@ -2193,7 +2209,7 @@
       <c r="J38" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="K38" s="11" t="s">
+      <c r="K38" s="5" t="s">
         <v>127</v>
       </c>
       <c r="L38" s="12"/>
@@ -2223,7 +2239,7 @@
       <c r="J39" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="K39" s="11" t="s">
+      <c r="K39" s="5" t="s">
         <v>150</v>
       </c>
       <c r="L39" s="12"/>
@@ -2253,7 +2269,7 @@
       <c r="J40" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="K40" s="11" t="s">
+      <c r="K40" s="5" t="s">
         <v>153</v>
       </c>
       <c r="L40" s="12"/>
@@ -2283,7 +2299,7 @@
       <c r="J41" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="K41" s="11" t="s">
+      <c r="K41" s="5" t="s">
         <v>150</v>
       </c>
       <c r="L41" s="12"/>
@@ -2313,7 +2329,7 @@
       <c r="J42" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="K42" s="11" t="s">
+      <c r="K42" s="5" t="s">
         <v>158</v>
       </c>
       <c r="L42" s="12"/>
@@ -2341,7 +2357,7 @@
       <c r="J43" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="K43" s="11"/>
+      <c r="K43" s="19"/>
       <c r="L43" s="12"/>
       <c r="M43" s="13"/>
     </row>
@@ -2367,7 +2383,7 @@
       <c r="J44" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="K44" s="11"/>
+      <c r="K44" s="19"/>
       <c r="L44" s="12"/>
       <c r="M44" s="13"/>
     </row>
@@ -2389,7 +2405,7 @@
         <v>150</v>
       </c>
       <c r="J45" s="10"/>
-      <c r="K45" s="11"/>
+      <c r="K45" s="19"/>
       <c r="L45" s="12"/>
       <c r="M45" s="13"/>
     </row>
@@ -2411,7 +2427,7 @@
         <v>153</v>
       </c>
       <c r="J46" s="10"/>
-      <c r="K46" s="11"/>
+      <c r="K46" s="19"/>
       <c r="L46" s="12"/>
       <c r="M46" s="13"/>
     </row>
@@ -2433,7 +2449,7 @@
         <v>161</v>
       </c>
       <c r="J47" s="10"/>
-      <c r="K47" s="11"/>
+      <c r="K47" s="19"/>
       <c r="L47" s="12"/>
       <c r="M47" s="13"/>
     </row>
@@ -3200,7 +3216,6 @@
       </c>
       <c r="I106" s="9"/>
       <c r="J106" s="10"/>
-      <c r="K106" s="11"/>
       <c r="L106" s="12"/>
       <c r="M106" s="13"/>
     </row>
@@ -3213,7 +3228,6 @@
       </c>
       <c r="I107" s="9"/>
       <c r="J107" s="10"/>
-      <c r="K107" s="11"/>
       <c r="L107" s="12"/>
       <c r="M107" s="13"/>
     </row>
@@ -3226,7 +3240,6 @@
       </c>
       <c r="I108" s="9"/>
       <c r="J108" s="10"/>
-      <c r="K108" s="11"/>
       <c r="L108" s="12"/>
       <c r="M108" s="13"/>
     </row>
@@ -3239,7 +3252,6 @@
       </c>
       <c r="I109" s="9"/>
       <c r="J109" s="10"/>
-      <c r="K109" s="11"/>
       <c r="L109" s="12"/>
       <c r="M109" s="13"/>
     </row>
@@ -3252,7 +3264,6 @@
       </c>
       <c r="I110" s="9"/>
       <c r="J110" s="10"/>
-      <c r="K110" s="11"/>
       <c r="L110" s="12"/>
       <c r="M110" s="13"/>
     </row>
@@ -3265,7 +3276,6 @@
       </c>
       <c r="I111" s="9"/>
       <c r="J111" s="10"/>
-      <c r="K111" s="11"/>
       <c r="L111" s="12"/>
       <c r="M111" s="13"/>
     </row>
@@ -3278,7 +3288,6 @@
       </c>
       <c r="I112" s="9"/>
       <c r="J112" s="10"/>
-      <c r="K112" s="11"/>
       <c r="L112" s="12"/>
       <c r="M112" s="13"/>
     </row>
@@ -3291,7 +3300,6 @@
       </c>
       <c r="I113" s="9"/>
       <c r="J113" s="10"/>
-      <c r="K113" s="11"/>
       <c r="L113" s="12"/>
       <c r="M113" s="13"/>
     </row>
@@ -3304,7 +3312,6 @@
       </c>
       <c r="I114" s="9"/>
       <c r="J114" s="10"/>
-      <c r="K114" s="11"/>
       <c r="L114" s="12"/>
       <c r="M114" s="13"/>
     </row>
@@ -3317,7 +3324,6 @@
       </c>
       <c r="I115" s="9"/>
       <c r="J115" s="10"/>
-      <c r="K115" s="11"/>
       <c r="L115" s="12"/>
       <c r="M115" s="13"/>
     </row>
@@ -3330,7 +3336,6 @@
       </c>
       <c r="I116" s="9"/>
       <c r="J116" s="10"/>
-      <c r="K116" s="11"/>
       <c r="L116" s="12"/>
       <c r="M116" s="13"/>
     </row>
@@ -3343,7 +3348,6 @@
       </c>
       <c r="I117" s="9"/>
       <c r="J117" s="10"/>
-      <c r="K117" s="11"/>
       <c r="L117" s="12"/>
       <c r="M117" s="13"/>
     </row>
@@ -3356,7 +3360,6 @@
       </c>
       <c r="I118" s="9"/>
       <c r="J118" s="10"/>
-      <c r="K118" s="11"/>
       <c r="L118" s="12"/>
       <c r="M118" s="13"/>
     </row>
@@ -3369,7 +3372,6 @@
       </c>
       <c r="I119" s="9"/>
       <c r="J119" s="10"/>
-      <c r="K119" s="11"/>
       <c r="L119" s="12"/>
       <c r="M119" s="13"/>
     </row>
@@ -3382,7 +3384,6 @@
       </c>
       <c r="I120" s="9"/>
       <c r="J120" s="10"/>
-      <c r="K120" s="11"/>
       <c r="L120" s="12"/>
       <c r="M120" s="13"/>
     </row>
@@ -3395,7 +3396,6 @@
       </c>
       <c r="I121" s="9"/>
       <c r="J121" s="10"/>
-      <c r="K121" s="11"/>
       <c r="L121" s="12"/>
       <c r="M121" s="13"/>
     </row>
@@ -3408,7 +3408,6 @@
       </c>
       <c r="I122" s="9"/>
       <c r="J122" s="10"/>
-      <c r="K122" s="11"/>
       <c r="L122" s="12"/>
       <c r="M122" s="13"/>
     </row>
@@ -3421,7 +3420,6 @@
       </c>
       <c r="I123" s="9"/>
       <c r="J123" s="10"/>
-      <c r="K123" s="11"/>
       <c r="L123" s="12"/>
       <c r="M123" s="13"/>
     </row>
@@ -3434,7 +3432,6 @@
       </c>
       <c r="I124" s="9"/>
       <c r="J124" s="10"/>
-      <c r="K124" s="11"/>
       <c r="L124" s="12"/>
       <c r="M124" s="13"/>
     </row>
@@ -3447,7 +3444,6 @@
       </c>
       <c r="I125" s="9"/>
       <c r="J125" s="10"/>
-      <c r="K125" s="11"/>
       <c r="L125" s="12"/>
       <c r="M125" s="13"/>
     </row>
@@ -3460,7 +3456,6 @@
       </c>
       <c r="I126" s="9"/>
       <c r="J126" s="10"/>
-      <c r="K126" s="11"/>
       <c r="L126" s="12"/>
       <c r="M126" s="13"/>
     </row>
@@ -3473,7 +3468,6 @@
       </c>
       <c r="I127" s="9"/>
       <c r="J127" s="10"/>
-      <c r="K127" s="11"/>
       <c r="L127" s="12"/>
       <c r="M127" s="13"/>
     </row>
@@ -3486,7 +3480,6 @@
       </c>
       <c r="I128" s="9"/>
       <c r="J128" s="10"/>
-      <c r="K128" s="11"/>
       <c r="L128" s="12"/>
       <c r="M128" s="13"/>
     </row>
@@ -3499,7 +3492,6 @@
       </c>
       <c r="I129" s="9"/>
       <c r="J129" s="10"/>
-      <c r="K129" s="11"/>
       <c r="L129" s="12"/>
       <c r="M129" s="13"/>
     </row>
@@ -3512,7 +3504,6 @@
       </c>
       <c r="I130" s="9"/>
       <c r="J130" s="10"/>
-      <c r="K130" s="11"/>
       <c r="L130" s="12"/>
       <c r="M130" s="13"/>
     </row>
@@ -3525,7 +3516,6 @@
       </c>
       <c r="I131" s="9"/>
       <c r="J131" s="10"/>
-      <c r="K131" s="11"/>
       <c r="L131" s="12"/>
       <c r="M131" s="13"/>
     </row>
@@ -3538,7 +3528,6 @@
       </c>
       <c r="I132" s="9"/>
       <c r="J132" s="10"/>
-      <c r="K132" s="11"/>
       <c r="L132" s="12"/>
       <c r="M132" s="13"/>
     </row>
@@ -3551,7 +3540,6 @@
       </c>
       <c r="I133" s="9"/>
       <c r="J133" s="10"/>
-      <c r="K133" s="11"/>
       <c r="L133" s="12"/>
       <c r="M133" s="13"/>
     </row>
@@ -3564,7 +3552,6 @@
       </c>
       <c r="I134" s="9"/>
       <c r="J134" s="10"/>
-      <c r="K134" s="11"/>
       <c r="L134" s="12"/>
       <c r="M134" s="13"/>
     </row>
@@ -3577,7 +3564,6 @@
       </c>
       <c r="I135" s="9"/>
       <c r="J135" s="10"/>
-      <c r="K135" s="11"/>
       <c r="L135" s="12"/>
     </row>
     <row r="136" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3589,7 +3575,6 @@
       </c>
       <c r="I136" s="9"/>
       <c r="J136" s="10"/>
-      <c r="K136" s="11"/>
       <c r="L136" s="12"/>
     </row>
     <row r="137" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3601,7 +3586,6 @@
       </c>
       <c r="I137" s="9"/>
       <c r="J137" s="10"/>
-      <c r="K137" s="11"/>
       <c r="L137" s="12"/>
     </row>
     <row r="138" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3613,7 +3597,6 @@
       </c>
       <c r="I138" s="9"/>
       <c r="J138" s="10"/>
-      <c r="K138" s="11"/>
       <c r="L138" s="12"/>
     </row>
     <row r="139" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3625,7 +3608,6 @@
       </c>
       <c r="I139" s="9"/>
       <c r="J139" s="10"/>
-      <c r="K139" s="11"/>
       <c r="L139" s="12"/>
     </row>
     <row r="140" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3637,7 +3619,6 @@
       </c>
       <c r="I140" s="9"/>
       <c r="J140" s="10"/>
-      <c r="K140" s="11"/>
       <c r="L140" s="12"/>
     </row>
     <row r="141" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3649,7 +3630,6 @@
       </c>
       <c r="I141" s="9"/>
       <c r="J141" s="10"/>
-      <c r="K141" s="11"/>
       <c r="L141" s="12"/>
     </row>
     <row r="142" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3661,7 +3641,6 @@
       </c>
       <c r="I142" s="9"/>
       <c r="J142" s="10"/>
-      <c r="K142" s="11"/>
       <c r="L142" s="12"/>
     </row>
     <row r="143" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3673,7 +3652,6 @@
       </c>
       <c r="I143" s="9"/>
       <c r="J143" s="10"/>
-      <c r="K143" s="11"/>
     </row>
     <row r="144" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A144" s="17" t="s">

</xml_diff>